<commit_message>
copy function template and more items in the excel table zu generate, add the rights to grant
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/MReusche cre Tab Interpolar Vorschlag.xlsx
+++ b/Postgres-cds_hub/init/template/MReusche cre Tab Interpolar Vorschlag.xlsx
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Parameter</t>
   </si>
@@ -115,12 +115,6 @@
     <t>Template</t>
   </si>
   <si>
-    <t>Berechtigung</t>
-  </si>
-  <si>
-    <t>Funktionsname</t>
-  </si>
-  <si>
     <t>01_main_user_schema_sequence.sql</t>
   </si>
   <si>
@@ -142,18 +136,12 @@
     <t>12_cre_table_raw_db_log.sql</t>
   </si>
   <si>
-    <t>14_cre_table_typ_log.sql</t>
-  </si>
-  <si>
     <t>keine</t>
   </si>
   <si>
     <t>SELECT</t>
   </si>
   <si>
-    <t>16_cre_table_typ_cds2db_in.sql</t>
-  </si>
-  <si>
     <t>18_cre_view_raw_type_diff_log.sql</t>
   </si>
   <si>
@@ -166,12 +154,6 @@
     <t>30_cds_in_to_db_log.sql</t>
   </si>
   <si>
-    <t>R_copy_fkt</t>
-  </si>
-  <si>
-    <t>do_cds_in_to_db_log</t>
-  </si>
-  <si>
     <t>50_frontend_out_views.sql</t>
   </si>
   <si>
@@ -184,9 +166,6 @@
     <t>TARGET_USER</t>
   </si>
   <si>
-    <t>GRANT_SCHEMA_NAME</t>
-  </si>
-  <si>
     <t>SEQ_NAME</t>
   </si>
   <si>
@@ -197,6 +176,39 @@
   </si>
   <si>
     <t>SCRIPTNAME</t>
+  </si>
+  <si>
+    <t>RIGHTS</t>
+  </si>
+  <si>
+    <t>CFF_POSTFIX</t>
+  </si>
+  <si>
+    <t>COPY_FUNC_SCRIPT_NAME</t>
+  </si>
+  <si>
+    <t>COPY_FUNC_NAME</t>
+  </si>
+  <si>
+    <t>COPY_FUNC_FROM_SCHEMA</t>
+  </si>
+  <si>
+    <t>TARGET_SCHEMA</t>
+  </si>
+  <si>
+    <t>31_cds_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>copy_raw_cds_in_to_db_log</t>
+  </si>
+  <si>
+    <t>copy_type_cds_in_to_db_log</t>
+  </si>
+  <si>
+    <t>14_cre_table_typ_cds2db_in.sql</t>
+  </si>
+  <si>
+    <t>16_cre_table_typ_log.sql</t>
   </si>
 </sst>
 </file>
@@ -225,7 +237,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +247,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -251,9 +269,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -312,11 +331,6 @@
         </row>
       </sheetData>
       <sheetData sheetId="3">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>db</v>
-          </cell>
-        </row>
         <row r="4">
           <cell r="A4" t="str">
             <v>db_log</v>
@@ -618,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,60 +649,71 @@
     <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.28515625" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" customWidth="1"/>
+    <col min="12" max="12" width="29.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
       <c r="C4" t="str">
         <f>'[1]1 User'!$A$3</f>
@@ -699,35 +724,35 @@
         <v>cds2db_in</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G4" t="str">
         <f>'[1]2 Schema'!B5</f>
         <v>cds2db_in_seq</v>
       </c>
       <c r="H4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I4" t="str">
         <f>'[1]1 User'!$A$3</f>
         <v>cds2db_user</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I5" t="str">
         <f>'[1]1 User'!$A$6</f>
         <v>db_user</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" t="str">
         <f>'[1]1 User'!$A$7</f>
@@ -738,172 +763,172 @@
         <v>db_log</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G6" t="str">
         <f>'[1]2 Schema'!$B$4</f>
         <v>db_log_seq</v>
       </c>
       <c r="H6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I6" t="str">
         <f>'[1]1 User'!$A$7</f>
         <v>db_log_user</v>
       </c>
-      <c r="J6" t="str">
-        <f>A15</f>
-        <v>30_cds_in_to_db_log.sql</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" t="str">
+        <f>'[1]2 Schema'!$A$5</f>
+        <v>cds2db_in</v>
+      </c>
+      <c r="M6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I7" t="str">
         <f>'[1]1 User'!$A$6</f>
         <v>db_user</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="str">
+        <f>'[1]1 User'!$A$3</f>
+        <v>cds2db_user</v>
+      </c>
+      <c r="D8" t="str">
+        <f>'[1]2 Schema'!$A$5</f>
+        <v>cds2db_in</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="str">
-        <f>'[1]1 User'!$A$7</f>
-        <v>db_log_user</v>
-      </c>
-      <c r="D8" t="str">
-        <f>'[1]2 Schema'!$A$4</f>
-        <v>db_log</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>9</v>
-      </c>
       <c r="I8" t="str">
-        <f>'[1]1 User'!$A$7</f>
-        <v>db_log_user</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <f>'[1]1 User'!$A$3</f>
+        <v>cds2db_user</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I9" t="str">
         <f>'[1]1 User'!$A$6</f>
         <v>db_user</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="str">
+        <f>'[1]1 User'!$A$7</f>
+        <v>db_log_user</v>
+      </c>
+      <c r="D10" t="str">
+        <f>'[1]2 Schema'!$A$4</f>
+        <v>db_log</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I10" t="str">
+        <f>'[1]1 User'!$A$7</f>
+        <v>db_log_user</v>
+      </c>
+      <c r="J10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" t="str">
+        <f>'[1]2 Schema'!$A$5</f>
+        <v>cds2db_in</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" t="str">
+        <f>'[1]1 User'!$A$6</f>
+        <v>db_user</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="str">
         <f>'[1]1 User'!$A$3</f>
         <v>cds2db_user</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="str">
+    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="str">
         <f>'[1]1 User'!$A$3</f>
         <v>cds2db_user</v>
       </c>
-      <c r="D11" t="str">
-        <f>'[1]2 Schema'!$A$5</f>
-        <v>cds2db_in</v>
-      </c>
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" t="str">
+      <c r="D13" s="2" t="str">
+        <f>'[1]2 Schema'!$A$6</f>
+        <v>cds2db_out</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="2" t="str">
         <f>'[1]1 User'!$A$3</f>
         <v>cds2db_user</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" t="str">
+    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="2" t="str">
         <f>'[1]1 User'!$A$6</f>
         <v>db_user</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>16</v>
-      </c>
-      <c r="C13" t="str">
-        <f>'[1]1 User'!$A$3</f>
-        <v>cds2db_user</v>
-      </c>
-      <c r="D13" t="str">
-        <f>'[1]2 Schema'!$A$6</f>
-        <v>cds2db_out</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" t="str">
-        <f>'[1]1 User'!$A$3</f>
-        <v>cds2db_user</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" t="str">
-        <f>'[1]1 User'!$A$6</f>
-        <v>db_user</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="str">
-        <f>'[1]1 User'!$A$6</f>
-        <v>db_user</v>
-      </c>
-      <c r="D15" t="str">
-        <f>'[1]2 Schema'!$A$2</f>
-        <v>db</v>
-      </c>
-      <c r="J15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>